<commit_message>
presupuesto se le agregaron contenido e informe contenido extra añadido
</commit_message>
<xml_diff>
--- a/presupuesto.xlsx
+++ b/presupuesto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARROQUIN\Desktop\P2_ORGA_G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7AE96D-C912-4A54-A300-26853492B3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBF6109-9F17-4723-915F-CFC5C2D0F153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <r>
       <rPr>
@@ -130,50 +130,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>18 COMPUERTA LOGICA AND 74LS08</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>7 COMPUERTA LOGICA OR 74LS32</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>6 COMPUERTA LOGICA XNOR 74LS266</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>4 COMPUERTA LOGICA NOT 74LS04</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>3 PROTOBOARD</t>
     </r>
   </si>
@@ -277,10 +233,34 @@
     </r>
   </si>
   <si>
-    <t>OTROS</t>
-  </si>
-  <si>
     <t>2 DECODIFICADOR 7 SEGMENTOS 74LS48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 PROTOBOARD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 COMPUERTA LOGICA AND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 COMPUERTA LOGICA XOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 COMPUERTA LOGICA OR </t>
+  </si>
+  <si>
+    <t>18 COMPUERTA LOGICA AND</t>
+  </si>
+  <si>
+    <t>4 COMPUERTA LOGICA NOT</t>
+  </si>
+  <si>
+    <t>2 COMPUERTAS XOR</t>
+  </si>
+  <si>
+    <t>TOTAL ABSOLUTO</t>
+  </si>
+  <si>
+    <t>OTROS VARIOS</t>
   </si>
 </sst>
 </file>
@@ -737,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="28" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="28" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -817,8 +797,8 @@
     </row>
     <row r="8" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
+      <c r="B8" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="C8" s="8">
         <v>80</v>
@@ -826,8 +806,8 @@
     </row>
     <row r="9" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
+      <c r="B9" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="C9" s="8">
         <v>35</v>
@@ -835,8 +815,8 @@
     </row>
     <row r="10" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
+      <c r="B10" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="8">
         <v>72</v>
@@ -844,8 +824,8 @@
     </row>
     <row r="11" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
-        <v>11</v>
+      <c r="B11" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="8">
         <v>20</v>
@@ -854,7 +834,7 @@
     <row r="12" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C12" s="8">
         <v>102</v>
@@ -863,7 +843,7 @@
     <row r="13" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C13" s="8">
         <v>15</v>
@@ -872,7 +852,7 @@
     <row r="14" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C14" s="8">
         <v>15</v>
@@ -881,7 +861,7 @@
     <row r="15" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C15" s="8">
         <v>118.5</v>
@@ -890,7 +870,7 @@
     <row r="16" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C16" s="8">
         <f>SUM(C2:C15)</f>
@@ -902,7 +882,7 @@
         <v>45750</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C17" s="8">
         <v>68</v>
@@ -911,7 +891,7 @@
     <row r="18" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C18" s="8">
         <v>10</v>
@@ -920,7 +900,7 @@
     <row r="19" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C19" s="8">
         <v>22</v>
@@ -929,7 +909,7 @@
     <row r="20" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C20" s="8">
         <v>39</v>
@@ -938,7 +918,7 @@
     <row r="21" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C21" s="8">
         <f>SUM(C17:C20)</f>
@@ -950,7 +930,7 @@
         <v>45780</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C22" s="8">
         <v>44</v>
@@ -959,7 +939,7 @@
     <row r="23" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C23" s="8">
         <v>15</v>
@@ -968,7 +948,7 @@
     <row r="24" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C24" s="8">
         <v>35</v>
@@ -977,11 +957,53 @@
     <row r="25" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C25" s="8">
-        <f>SUM(C22:C24)</f>
-        <v>94</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="8">
+        <f>SUM(C22:C27)</f>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="8">
+        <f>C16+C21+C28</f>
+        <v>965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mejore el informe y agregue los gastos de hoy del presupuesto
</commit_message>
<xml_diff>
--- a/presupuesto.xlsx
+++ b/presupuesto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARROQUIN\Desktop\P2_ORGA_G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBF6109-9F17-4723-915F-CFC5C2D0F153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C82A0FE-B5FE-4760-A7E7-1E8A5F831453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <r>
       <rPr>
@@ -222,17 +222,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>7 COMPUERTA LÓGICA AND 74LS08</t>
-    </r>
-  </si>
-  <si>
     <t>2 DECODIFICADOR 7 SEGMENTOS 74LS48</t>
   </si>
   <si>
@@ -261,6 +250,18 @@
   </si>
   <si>
     <t>OTROS VARIOS</t>
+  </si>
+  <si>
+    <t>7 COMPUERTA LÓGICA AND 74LS08</t>
+  </si>
+  <si>
+    <t>5 COMPUERTA LÓGICA AND 74LS08</t>
+  </si>
+  <si>
+    <t>subtotal</t>
+  </si>
+  <si>
+    <t>Q</t>
   </si>
 </sst>
 </file>
@@ -271,7 +272,7 @@
     <numFmt numFmtId="8" formatCode="&quot;Q&quot;#,##0.00;[Red]\-&quot;Q&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="m/dd/yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -296,8 +297,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +315,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -389,21 +409,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -411,6 +422,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -717,36 +752,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="28" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="28" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
-    <col min="2" max="2" width="71.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="2" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="3">
         <v>45719</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="14">
         <v>120</v>
       </c>
     </row>
@@ -755,7 +792,7 @@
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="5">
         <v>11</v>
       </c>
     </row>
@@ -764,7 +801,7 @@
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="5">
         <v>14</v>
       </c>
     </row>
@@ -773,7 +810,7 @@
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="5">
         <v>22</v>
       </c>
     </row>
@@ -782,7 +819,7 @@
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="5">
         <v>20</v>
       </c>
     </row>
@@ -791,43 +828,43 @@
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="5">
         <v>7.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="B8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="B9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="8">
+      <c r="B10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="8">
+      <c r="B11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5">
         <v>20</v>
       </c>
     </row>
@@ -836,7 +873,7 @@
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="5">
         <v>102</v>
       </c>
     </row>
@@ -845,7 +882,7 @@
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="5">
         <v>15</v>
       </c>
     </row>
@@ -854,16 +891,16 @@
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="8">
+        <v>26</v>
+      </c>
+      <c r="C15" s="5">
         <v>118.5</v>
       </c>
     </row>
@@ -872,19 +909,19 @@
       <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="5">
         <f>SUM(C2:C15)</f>
         <v>652</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="3">
         <v>45750</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="15">
         <v>68</v>
       </c>
     </row>
@@ -893,16 +930,16 @@
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="8">
+      <c r="B19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="5">
         <v>22</v>
       </c>
     </row>
@@ -911,7 +948,7 @@
       <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="5">
         <v>39</v>
       </c>
     </row>
@@ -920,19 +957,19 @@
       <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="5">
         <f>SUM(C17:C20)</f>
         <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="3">
         <v>45780</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="15">
         <v>44</v>
       </c>
     </row>
@@ -941,43 +978,43 @@
       <c r="B23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="8">
+      <c r="B24" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="5">
         <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="8">
+        <v>18</v>
+      </c>
+      <c r="C25" s="5">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="8">
+        <v>19</v>
+      </c>
+      <c r="C26" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="8">
+        <v>24</v>
+      </c>
+      <c r="C27" s="5">
         <v>24</v>
       </c>
     </row>
@@ -986,24 +1023,49 @@
       <c r="B28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="5">
         <f>SUM(C22:C27)</f>
         <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="8"/>
+      <c r="A29" s="9">
+        <v>45722</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="15">
+        <v>25</v>
+      </c>
     </row>
     <row r="30" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2" t="s">
+      <c r="A30" s="8"/>
+      <c r="B30" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="8">
-        <f>C16+C21+C28</f>
-        <v>965</v>
+      <c r="C30" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="5">
+        <f>SUM(C29:C30)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="5">
+        <f>C16+C21+C28+C31</f>
+        <v>1015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>